<commit_message>
alk plot app working
</commit_message>
<xml_diff>
--- a/data/example_alk/alk_data/alk_2022.02.21_r1.xlsx
+++ b/data/example_alk/alk_data/alk_2022.02.21_r1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul.mcelhany/Documents/GitHub/alk_dic/data/example_alk/alk_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F2A45B-54C7-0645-9C15-E6465FCBB9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD85FF4-147D-D04A-9DF7-6356CC221E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3680" yWindow="4020" windowWidth="33820" windowHeight="17600" xr2:uid="{C3874D3F-43D9-FE47-BB0F-9142419DB1A0}"/>
   </bookViews>
@@ -191,10 +191,10 @@
     <t>pre_experiment</t>
   </si>
   <si>
+    <t>alk_lab</t>
+  </si>
+  <si>
     <t>nwfsc_oa</t>
-  </si>
-  <si>
-    <t>alk_lab</t>
   </si>
 </sst>
 </file>
@@ -558,7 +558,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F7"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,7 +570,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -673,7 +673,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
@@ -721,7 +721,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -771,7 +771,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>15</v>
@@ -819,7 +819,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>
@@ -867,7 +867,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>17</v>
@@ -915,7 +915,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>18</v>
@@ -965,7 +965,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>20</v>
@@ -1065,7 +1065,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>21</v>
@@ -1113,7 +1113,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="9">
+  <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D49" xr:uid="{0121CAD0-C233-2A41-992E-1591696CC270}">
       <formula1>"calcium_r1, alk_vs_sal"</formula1>
     </dataValidation>
@@ -1138,9 +1138,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I11" xr:uid="{AC156081-3CA2-DB47-8CF1-9D067647891F}">
       <formula1>"feed_day, pre_experiment, alk_vs_sal,standard"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A50" xr:uid="{D73B2671-A1A0-104F-BBFD-AA0F4D7CD917}">
-      <formula1>"nwfsc_oa, gagnon"</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
edits to alkalinity plot app
</commit_message>
<xml_diff>
--- a/data/example_alk/alk_data/alk_2022.02.21_r1.xlsx
+++ b/data/example_alk/alk_data/alk_2022.02.21_r1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul.mcelhany/Documents/GitHub/alk_dic/data/example_alk/alk_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD85FF4-147D-D04A-9DF7-6356CC221E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B674679-1589-914C-A79E-934BE159C1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3680" yWindow="4020" windowWidth="33820" windowHeight="17600" xr2:uid="{C3874D3F-43D9-FE47-BB0F-9142419DB1A0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="55">
   <si>
     <t>sample_id</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>nwfsc_oa</t>
+  </si>
+  <si>
+    <t>quality_flag</t>
   </si>
 </sst>
 </file>
@@ -555,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35BAF4BB-7371-304D-AD1D-093CC190A452}">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,7 +571,7 @@
     <col min="13" max="13" width="25.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -618,10 +621,13 @@
         <v>10</v>
       </c>
       <c r="Q1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -667,11 +673,14 @@
       <c r="P2" s="1">
         <v>5595.8</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="2">
+        <v>2</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -717,9 +726,12 @@
       <c r="P3" s="1">
         <v>5589.21</v>
       </c>
-      <c r="Q3" s="1"/>
+      <c r="Q3" s="2">
+        <v>2</v>
+      </c>
+      <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -765,11 +777,14 @@
       <c r="P4" s="1">
         <v>5588.29</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" s="2">
+        <v>2</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -815,9 +830,12 @@
       <c r="P5" s="1">
         <v>3087.25</v>
       </c>
-      <c r="Q5" s="1"/>
+      <c r="Q5" s="2">
+        <v>2</v>
+      </c>
+      <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -863,9 +881,12 @@
       <c r="P6" s="1">
         <v>3080.27</v>
       </c>
-      <c r="Q6" s="1"/>
+      <c r="Q6" s="2">
+        <v>2</v>
+      </c>
+      <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -911,9 +932,12 @@
       <c r="P7" s="1">
         <v>3077.52</v>
       </c>
-      <c r="Q7" s="1"/>
+      <c r="Q7" s="2">
+        <v>2</v>
+      </c>
+      <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -959,11 +983,14 @@
       <c r="P8" s="1">
         <v>3144.62</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="2">
+        <v>2</v>
+      </c>
+      <c r="R8" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1009,11 +1036,14 @@
       <c r="P9" s="1">
         <v>3148.85</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" s="2">
+        <v>2</v>
+      </c>
+      <c r="R9" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -1059,11 +1089,14 @@
       <c r="P10" s="1">
         <v>3095.63</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" s="2">
+        <v>1</v>
+      </c>
+      <c r="R10" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1107,7 +1140,10 @@
         <v>136.9</v>
       </c>
       <c r="P11" s="1"/>
-      <c r="Q11" s="1" t="s">
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>